<commit_message>
Complete total distribution; Choose the 3 labels
</commit_message>
<xml_diff>
--- a/Database.xlsx
+++ b/Database.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uniofnottm.sharepoint.com/sites/WoZing-Machine/Shared Documents/Deliverable/SortingTask/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chenyu/machine_learning/rl/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="212" documentId="8_{E652683B-E3C0-C742-B92C-EBA5655DAF2A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{1DAE9A2A-91CE-9347-94C7-72B0BB05B152}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A19A702-310B-D44A-8F97-C122F1465B7F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="19980" firstSheet="5" activeTab="5" xr2:uid="{DBC0DE7E-C58B-064F-B6FB-B328F19F6478}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="2" xr2:uid="{DBC0DE7E-C58B-064F-B6FB-B328F19F6478}"/>
   </bookViews>
   <sheets>
     <sheet name="baskets" sheetId="5" r:id="rId1"/>
@@ -20,7 +20,7 @@
     <sheet name="participants" sheetId="1" r:id="rId5"/>
     <sheet name="sorts" sheetId="6" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="191028" calcCompleted="0"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -12144,12 +12144,19 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="等线"/>
+      <family val="3"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -12184,7 +12191,7 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="30">
     <dxf>
@@ -12419,7 +12426,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -12721,21 +12728,21 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.95"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
   <cols>
     <col min="5" max="5" width="39" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="71.125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="25.125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="20.375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="19.625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="26.625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="23.125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="71.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="25.1640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="26.6640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="23.1640625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="17.5" style="1" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="16" style="1" customWidth="1"/>
-    <col min="15" max="15" width="19.125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="19.1640625" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="89" bestFit="1" customWidth="1"/>
-    <col min="17" max="18" width="30.375" bestFit="1" customWidth="1"/>
+    <col min="17" max="18" width="30.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18">
@@ -17003,6 +17010,7 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
@@ -17018,9 +17026,9 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.95"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
   <cols>
-    <col min="2" max="2" width="12.875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -17128,6 +17136,7 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
@@ -17139,19 +17148,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{648D499E-EE43-E743-BA4F-43823CD30818}">
   <dimension ref="A1:K167"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.95"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
   <cols>
-    <col min="2" max="2" width="17.125" customWidth="1"/>
-    <col min="4" max="5" width="33.125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.1640625" customWidth="1"/>
+    <col min="4" max="5" width="33.1640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="37.5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="33.125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="45.625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="33.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="45.6640625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="26" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="17.125" style="1" customWidth="1"/>
+    <col min="10" max="10" width="17.1640625" style="1" customWidth="1"/>
     <col min="11" max="11" width="16.5" customWidth="1"/>
   </cols>
   <sheetData>
@@ -20838,6 +20847,7 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
@@ -20853,9 +20863,9 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.95"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
   <cols>
-    <col min="2" max="2" width="18.875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.83203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="21" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -21047,6 +21057,7 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
@@ -21062,14 +21073,14 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.95"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
   <cols>
     <col min="4" max="4" width="21.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.875" customWidth="1"/>
+    <col min="5" max="5" width="18.83203125" customWidth="1"/>
     <col min="6" max="6" width="36.5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="35.375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="35.33203125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="36.5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
@@ -21959,6 +21970,7 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
@@ -21970,29 +21982,29 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B7D1BAD-DDCF-2649-8D4E-D52652111315}">
   <dimension ref="A1:Y631"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="200" workbookViewId="0">
-      <selection activeCell="E632" sqref="E632"/>
+    <sheetView zoomScaleNormal="200" workbookViewId="0">
+      <selection activeCell="B44" sqref="B44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.95"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
   <cols>
-    <col min="6" max="6" width="19.125" style="3" customWidth="1"/>
-    <col min="7" max="7" width="18.375" style="3" customWidth="1"/>
-    <col min="8" max="9" width="20.875" customWidth="1"/>
-    <col min="10" max="10" width="44.625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.1640625" style="3" customWidth="1"/>
+    <col min="7" max="7" width="18.33203125" style="3" customWidth="1"/>
+    <col min="8" max="9" width="20.83203125" customWidth="1"/>
+    <col min="10" max="10" width="44.6640625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="21.625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="32.875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="21.6640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="32.83203125" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="14" customWidth="1"/>
     <col min="15" max="15" width="15.5" customWidth="1"/>
     <col min="16" max="16" width="18" customWidth="1"/>
-    <col min="19" max="19" width="12.625" customWidth="1"/>
-    <col min="20" max="20" width="12.125" customWidth="1"/>
-    <col min="21" max="21" width="17.375" customWidth="1"/>
+    <col min="19" max="19" width="12.6640625" customWidth="1"/>
+    <col min="20" max="20" width="12.1640625" customWidth="1"/>
+    <col min="21" max="21" width="17.33203125" customWidth="1"/>
     <col min="22" max="22" width="17.5" customWidth="1"/>
-    <col min="23" max="23" width="16.875" customWidth="1"/>
+    <col min="23" max="23" width="16.83203125" customWidth="1"/>
     <col min="24" max="24" width="22" customWidth="1"/>
-    <col min="25" max="25" width="33.625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="33.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:25">
@@ -55279,6 +55291,7 @@
       <c r="Y631" s="3"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
@@ -55478,12 +55491,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -55492,14 +55499,44 @@
 </FormTemplates>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{695739D6-B888-44E4-A57A-F8AFB8873FBE}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{695739D6-B888-44E4-A57A-F8AFB8873FBE}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="f39798f5-29e1-414d-b589-639498489584"/>
+    <ds:schemaRef ds:uri="ed24df7a-2896-4dd2-8b73-5f08fa70715e"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{21F136AE-F8AF-47D1-925F-18FC59BE60A3}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BCC787E2-6A7D-46CB-BABB-385C4AC74EA0}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BCC787E2-6A7D-46CB-BABB-385C4AC74EA0}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{21F136AE-F8AF-47D1-925F-18FC59BE60A3}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Store sorting info as dict
</commit_message>
<xml_diff>
--- a/Database.xlsx
+++ b/Database.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11208"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chenyu/machine_learning/rl/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A19A702-310B-D44A-8F97-C122F1465B7F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6983CD86-E68F-C345-AE23-E916D374474D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="2" xr2:uid="{DBC0DE7E-C58B-064F-B6FB-B328F19F6478}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="5" xr2:uid="{DBC0DE7E-C58B-064F-B6FB-B328F19F6478}"/>
   </bookViews>
   <sheets>
     <sheet name="baskets" sheetId="5" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9933" uniqueCount="4034">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9933" uniqueCount="4035">
   <si>
     <t>b_id</t>
   </si>
@@ -12138,6 +12138,10 @@
   </si>
   <si>
     <t>don't remember</t>
+  </si>
+  <si>
+    <t>1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -12388,9 +12392,9 @@
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{DB8707D2-FEE1-154B-AB93-0E5D03DE31CD}" name="Table1" displayName="Table1" ref="A1:Y631" totalsRowShown="0" dataDxfId="25">
   <autoFilter ref="A1:Y631" xr:uid="{07C1E760-0F0C-3542-AF05-24DC0F24D3F0}">
-    <filterColumn colId="2">
+    <filterColumn colId="1">
       <filters>
-        <filter val="1"/>
+        <filter val="11"/>
       </filters>
     </filterColumn>
   </autoFilter>
@@ -17148,7 +17152,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{648D499E-EE43-E743-BA4F-43823CD30818}">
   <dimension ref="A1:K167"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -20859,7 +20863,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B26EC24-E353-1747-9011-29FA4CE28EDA}">
   <dimension ref="A1:C17"/>
   <sheetViews>
-    <sheetView topLeftCell="T1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -21982,8 +21986,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B7D1BAD-DDCF-2649-8D4E-D52652111315}">
   <dimension ref="A1:Y631"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="200" workbookViewId="0">
-      <selection activeCell="B44" sqref="B44"/>
+    <sheetView tabSelected="1" zoomScaleNormal="200" workbookViewId="0">
+      <selection activeCell="C637" sqref="C637"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
@@ -22084,7 +22088,7 @@
         <v>1053</v>
       </c>
     </row>
-    <row r="2" spans="1:25">
+    <row r="2" spans="1:25" hidden="1">
       <c r="A2" s="3" t="s">
         <v>1054</v>
       </c>
@@ -23163,7 +23167,7 @@
       <c r="X22" s="3"/>
       <c r="Y22" s="3"/>
     </row>
-    <row r="23" spans="1:25">
+    <row r="23" spans="1:25" hidden="1">
       <c r="A23" s="3" t="s">
         <v>1168</v>
       </c>
@@ -24208,7 +24212,7 @@
       <c r="X43" s="3"/>
       <c r="Y43" s="3"/>
     </row>
-    <row r="44" spans="1:25">
+    <row r="44" spans="1:25" hidden="1">
       <c r="A44" s="3" t="s">
         <v>1272</v>
       </c>
@@ -25311,7 +25315,7 @@
       </c>
       <c r="Y64" s="3"/>
     </row>
-    <row r="65" spans="1:25">
+    <row r="65" spans="1:25" hidden="1">
       <c r="A65" s="3" t="s">
         <v>1388</v>
       </c>
@@ -26392,7 +26396,7 @@
       <c r="X85" s="3"/>
       <c r="Y85" s="3"/>
     </row>
-    <row r="86" spans="1:25">
+    <row r="86" spans="1:25" hidden="1">
       <c r="A86" s="3" t="s">
         <v>1495</v>
       </c>
@@ -27471,7 +27475,7 @@
       <c r="X106" s="3"/>
       <c r="Y106" s="3"/>
     </row>
-    <row r="107" spans="1:25">
+    <row r="107" spans="1:25" hidden="1">
       <c r="A107" s="3" t="s">
         <v>1601</v>
       </c>
@@ -28562,7 +28566,7 @@
       <c r="X127" s="3"/>
       <c r="Y127" s="3"/>
     </row>
-    <row r="128" spans="1:25">
+    <row r="128" spans="1:25" hidden="1">
       <c r="A128" s="3" t="s">
         <v>1700</v>
       </c>
@@ -29651,7 +29655,7 @@
       <c r="X148" s="3"/>
       <c r="Y148" s="3"/>
     </row>
-    <row r="149" spans="1:25">
+    <row r="149" spans="1:25" hidden="1">
       <c r="A149" s="3" t="s">
         <v>1799</v>
       </c>
@@ -30746,7 +30750,7 @@
       <c r="X169" s="3"/>
       <c r="Y169" s="3"/>
     </row>
-    <row r="170" spans="1:25">
+    <row r="170" spans="1:25" hidden="1">
       <c r="A170" s="3" t="s">
         <v>1892</v>
       </c>
@@ -31819,7 +31823,7 @@
       </c>
       <c r="Y190" s="3"/>
     </row>
-    <row r="191" spans="1:25">
+    <row r="191" spans="1:25" hidden="1">
       <c r="A191" s="3" t="s">
         <v>1987</v>
       </c>
@@ -32954,7 +32958,7 @@
       </c>
       <c r="Y211" s="3"/>
     </row>
-    <row r="212" spans="1:25" hidden="1">
+    <row r="212" spans="1:25">
       <c r="A212" s="3" t="s">
         <v>2084</v>
       </c>
@@ -32962,7 +32966,7 @@
         <v>1100</v>
       </c>
       <c r="C212" s="3" t="s">
-        <v>2085</v>
+        <v>4034</v>
       </c>
       <c r="D212" s="3" t="s">
         <v>1290</v>
@@ -33009,7 +33013,7 @@
       </c>
       <c r="Y212" s="3"/>
     </row>
-    <row r="213" spans="1:25" hidden="1">
+    <row r="213" spans="1:25">
       <c r="A213" s="3" t="s">
         <v>2090</v>
       </c>
@@ -33062,7 +33066,7 @@
       </c>
       <c r="Y213" s="3"/>
     </row>
-    <row r="214" spans="1:25" hidden="1">
+    <row r="214" spans="1:25">
       <c r="A214" s="3" t="s">
         <v>2094</v>
       </c>
@@ -33115,7 +33119,7 @@
       <c r="X214" s="3"/>
       <c r="Y214" s="3"/>
     </row>
-    <row r="215" spans="1:25" hidden="1">
+    <row r="215" spans="1:25">
       <c r="A215" s="3" t="s">
         <v>2098</v>
       </c>
@@ -33168,7 +33172,7 @@
       <c r="X215" s="3"/>
       <c r="Y215" s="3"/>
     </row>
-    <row r="216" spans="1:25" hidden="1">
+    <row r="216" spans="1:25">
       <c r="A216" s="3" t="s">
         <v>2103</v>
       </c>
@@ -33221,7 +33225,7 @@
       </c>
       <c r="Y216" s="3"/>
     </row>
-    <row r="217" spans="1:25" hidden="1">
+    <row r="217" spans="1:25">
       <c r="A217" s="3" t="s">
         <v>2109</v>
       </c>
@@ -33272,7 +33276,7 @@
       </c>
       <c r="Y217" s="3"/>
     </row>
-    <row r="218" spans="1:25" hidden="1">
+    <row r="218" spans="1:25">
       <c r="A218" s="3" t="s">
         <v>2115</v>
       </c>
@@ -33325,7 +33329,7 @@
       </c>
       <c r="Y218" s="3"/>
     </row>
-    <row r="219" spans="1:25" hidden="1">
+    <row r="219" spans="1:25">
       <c r="A219" s="3" t="s">
         <v>2120</v>
       </c>
@@ -33378,7 +33382,7 @@
       </c>
       <c r="Y219" s="3"/>
     </row>
-    <row r="220" spans="1:25" hidden="1">
+    <row r="220" spans="1:25">
       <c r="A220" s="3" t="s">
         <v>2125</v>
       </c>
@@ -33429,7 +33433,7 @@
       <c r="X220" s="3"/>
       <c r="Y220" s="3"/>
     </row>
-    <row r="221" spans="1:25" hidden="1">
+    <row r="221" spans="1:25">
       <c r="A221" s="3" t="s">
         <v>2129</v>
       </c>
@@ -33484,7 +33488,7 @@
       </c>
       <c r="Y221" s="3"/>
     </row>
-    <row r="222" spans="1:25" hidden="1">
+    <row r="222" spans="1:25">
       <c r="A222" s="3" t="s">
         <v>2133</v>
       </c>
@@ -33539,7 +33543,7 @@
         <v>2138</v>
       </c>
     </row>
-    <row r="223" spans="1:25" hidden="1">
+    <row r="223" spans="1:25">
       <c r="A223" s="3" t="s">
         <v>2139</v>
       </c>
@@ -33588,7 +33592,7 @@
       </c>
       <c r="Y223" s="3"/>
     </row>
-    <row r="224" spans="1:25" hidden="1">
+    <row r="224" spans="1:25">
       <c r="A224" s="3" t="s">
         <v>2144</v>
       </c>
@@ -33645,7 +33649,7 @@
       </c>
       <c r="Y224" s="3"/>
     </row>
-    <row r="225" spans="1:25" hidden="1">
+    <row r="225" spans="1:25">
       <c r="A225" s="3" t="s">
         <v>2151</v>
       </c>
@@ -33702,7 +33706,7 @@
       </c>
       <c r="Y225" s="3"/>
     </row>
-    <row r="226" spans="1:25" hidden="1">
+    <row r="226" spans="1:25">
       <c r="A226" s="3" t="s">
         <v>2156</v>
       </c>
@@ -33757,7 +33761,7 @@
       <c r="X226" s="3"/>
       <c r="Y226" s="3"/>
     </row>
-    <row r="227" spans="1:25" hidden="1">
+    <row r="227" spans="1:25">
       <c r="A227" s="3" t="s">
         <v>2161</v>
       </c>
@@ -33808,7 +33812,7 @@
       <c r="X227" s="3"/>
       <c r="Y227" s="3"/>
     </row>
-    <row r="228" spans="1:25" hidden="1">
+    <row r="228" spans="1:25">
       <c r="A228" s="3" t="s">
         <v>2166</v>
       </c>
@@ -33861,7 +33865,7 @@
       </c>
       <c r="Y228" s="3"/>
     </row>
-    <row r="229" spans="1:25" hidden="1">
+    <row r="229" spans="1:25">
       <c r="A229" s="3" t="s">
         <v>2172</v>
       </c>
@@ -33920,7 +33924,7 @@
       </c>
       <c r="Y229" s="3"/>
     </row>
-    <row r="230" spans="1:25" hidden="1">
+    <row r="230" spans="1:25">
       <c r="A230" s="3" t="s">
         <v>2179</v>
       </c>
@@ -33977,7 +33981,7 @@
       </c>
       <c r="Y230" s="3"/>
     </row>
-    <row r="231" spans="1:25" hidden="1">
+    <row r="231" spans="1:25">
       <c r="A231" s="3" t="s">
         <v>2188</v>
       </c>
@@ -34032,7 +34036,7 @@
       </c>
       <c r="Y231" s="3"/>
     </row>
-    <row r="232" spans="1:25" hidden="1">
+    <row r="232" spans="1:25">
       <c r="A232" s="3" t="s">
         <v>2194</v>
       </c>
@@ -34081,7 +34085,7 @@
       <c r="X232" s="3"/>
       <c r="Y232" s="3"/>
     </row>
-    <row r="233" spans="1:25">
+    <row r="233" spans="1:25" hidden="1">
       <c r="A233" s="3" t="s">
         <v>2199</v>
       </c>
@@ -35216,7 +35220,7 @@
       <c r="X253" s="3"/>
       <c r="Y253" s="3"/>
     </row>
-    <row r="254" spans="1:25">
+    <row r="254" spans="1:25" hidden="1">
       <c r="A254" s="3" t="s">
         <v>2298</v>
       </c>
@@ -36313,7 +36317,7 @@
       </c>
       <c r="Y274" s="3"/>
     </row>
-    <row r="275" spans="1:25">
+    <row r="275" spans="1:25" hidden="1">
       <c r="A275" s="3" t="s">
         <v>2404</v>
       </c>
@@ -37410,7 +37414,7 @@
       <c r="X295" s="3"/>
       <c r="Y295" s="3"/>
     </row>
-    <row r="296" spans="1:25">
+    <row r="296" spans="1:25" hidden="1">
       <c r="A296" s="3" t="s">
         <v>2504</v>
       </c>
@@ -38521,7 +38525,7 @@
       <c r="X316" s="3"/>
       <c r="Y316" s="3"/>
     </row>
-    <row r="317" spans="1:25">
+    <row r="317" spans="1:25" hidden="1">
       <c r="A317" s="3" t="s">
         <v>2604</v>
       </c>
@@ -39634,7 +39638,7 @@
       </c>
       <c r="Y337" s="3"/>
     </row>
-    <row r="338" spans="1:25">
+    <row r="338" spans="1:25" hidden="1">
       <c r="A338" s="3" t="s">
         <v>2692</v>
       </c>
@@ -40765,7 +40769,7 @@
       <c r="X358" s="3"/>
       <c r="Y358" s="3"/>
     </row>
-    <row r="359" spans="1:25">
+    <row r="359" spans="1:25" hidden="1">
       <c r="A359" s="3" t="s">
         <v>2774</v>
       </c>
@@ -41856,7 +41860,7 @@
       <c r="X379" s="3"/>
       <c r="Y379" s="3"/>
     </row>
-    <row r="380" spans="1:25">
+    <row r="380" spans="1:25" hidden="1">
       <c r="A380" s="3" t="s">
         <v>2868</v>
       </c>
@@ -42945,7 +42949,7 @@
       <c r="X400" s="3"/>
       <c r="Y400" s="3"/>
     </row>
-    <row r="401" spans="1:25">
+    <row r="401" spans="1:25" hidden="1">
       <c r="A401" s="3" t="s">
         <v>2965</v>
       </c>
@@ -44058,7 +44062,7 @@
       <c r="X421" s="3"/>
       <c r="Y421" s="3"/>
     </row>
-    <row r="422" spans="1:25">
+    <row r="422" spans="1:25" hidden="1">
       <c r="A422" s="3" t="s">
         <v>3050</v>
       </c>
@@ -45181,7 +45185,7 @@
       </c>
       <c r="Y442" s="3"/>
     </row>
-    <row r="443" spans="1:25">
+    <row r="443" spans="1:25" hidden="1">
       <c r="A443" s="3" t="s">
         <v>3148</v>
       </c>
@@ -46302,7 +46306,7 @@
       <c r="X463" s="3"/>
       <c r="Y463" s="3"/>
     </row>
-    <row r="464" spans="1:25">
+    <row r="464" spans="1:25" hidden="1">
       <c r="A464" s="3" t="s">
         <v>3250</v>
       </c>
@@ -47403,7 +47407,7 @@
       <c r="X484" s="3"/>
       <c r="Y484" s="3"/>
     </row>
-    <row r="485" spans="1:25">
+    <row r="485" spans="1:25" hidden="1">
       <c r="A485" s="3" t="s">
         <v>3346</v>
       </c>
@@ -48526,7 +48530,7 @@
       <c r="X505" s="3"/>
       <c r="Y505" s="3"/>
     </row>
-    <row r="506" spans="1:25">
+    <row r="506" spans="1:25" hidden="1">
       <c r="A506" s="3" t="s">
         <v>3465</v>
       </c>
@@ -49673,7 +49677,7 @@
       <c r="X526" s="3"/>
       <c r="Y526" s="3"/>
     </row>
-    <row r="527" spans="1:25">
+    <row r="527" spans="1:25" hidden="1">
       <c r="A527" s="3" t="s">
         <v>3579</v>
       </c>
@@ -50798,7 +50802,7 @@
       <c r="X547" s="3"/>
       <c r="Y547" s="3"/>
     </row>
-    <row r="548" spans="1:25">
+    <row r="548" spans="1:25" hidden="1">
       <c r="A548" s="3" t="s">
         <v>3666</v>
       </c>
@@ -51927,7 +51931,7 @@
       <c r="X568" s="3"/>
       <c r="Y568" s="3"/>
     </row>
-    <row r="569" spans="1:25">
+    <row r="569" spans="1:25" hidden="1">
       <c r="A569" s="3" t="s">
         <v>3760</v>
       </c>
@@ -53028,7 +53032,7 @@
       <c r="X589" s="3"/>
       <c r="Y589" s="3"/>
     </row>
-    <row r="590" spans="1:25">
+    <row r="590" spans="1:25" hidden="1">
       <c r="A590" s="3" t="s">
         <v>3841</v>
       </c>
@@ -54141,7 +54145,7 @@
       <c r="X610" s="3"/>
       <c r="Y610" s="3"/>
     </row>
-    <row r="611" spans="1:25">
+    <row r="611" spans="1:25" hidden="1">
       <c r="A611" s="3" t="s">
         <v>3948</v>
       </c>
@@ -55491,18 +55495,18 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -55525,18 +55529,18 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BCC787E2-6A7D-46CB-BABB-385C4AC74EA0}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{21F136AE-F8AF-47D1-925F-18FC59BE60A3}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BCC787E2-6A7D-46CB-BABB-385C4AC74EA0}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>